<commit_message>
Update Bill_of_materials_NOG NIET KLAAR.xlsx
</commit_message>
<xml_diff>
--- a/Bill_of_materials_NOG NIET KLAAR.xlsx
+++ b/Bill_of_materials_NOG NIET KLAAR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gijsj\Documents\1_EAI\Github\Elektronische-systemen-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1A80E6EF-8580-4A6C-973E-E25CF298BA06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76511066-1AD5-4F63-BB5A-2CD07ACDAA4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{23BF4C88-1078-42E7-9D0C-D5A36D1001D8}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
   <si>
     <t>Aantal</t>
   </si>
@@ -49,21 +49,9 @@
     <t>Website</t>
   </si>
   <si>
-    <t>MQ-3</t>
-  </si>
-  <si>
-    <t>weerstanden</t>
-  </si>
-  <si>
     <t>arduino nano</t>
   </si>
   <si>
-    <t>regelbare weerstand</t>
-  </si>
-  <si>
-    <t>ic</t>
-  </si>
-  <si>
     <t>led rood</t>
   </si>
   <si>
@@ -83,6 +71,75 @@
   </si>
   <si>
     <t>https://www.conrad.be/nl/p/vossloh-schwabe-ld-20-5mm-gn-bedrade-led-groen-rond-5-mm-40-mcd-60-20-ma-2-2-v-184705.html</t>
+  </si>
+  <si>
+    <t>https://be.farnell.com/multicomp/mcl053ad/led-5mm-36-orange/dp/1581141?st=oranje%20led</t>
+  </si>
+  <si>
+    <t>https://www.conrad.be/nl/p/arduino-nano-development-board-core-nano-atmega328-1172623.html</t>
+  </si>
+  <si>
+    <t>https://www.conrad.be/nl/p/vishay-t7ya101mt20-precisietrimmer-lineair-0-5-w-100-210-230-1-stuk-s-424366.html</t>
+  </si>
+  <si>
+    <t>Trimmer</t>
+  </si>
+  <si>
+    <t>https://www.conrad.be/nl/p/weltron-401951-vermogensweerstand-33-axiaal-bedraad-5-w-5-1-stuk-s-401951.html</t>
+  </si>
+  <si>
+    <t>https://www.conrad.be/nl/p/weltron-koolfilmweerstand-150-axiaal-bedraad-0411-0-5-w-5-1-stuk-s-405159.html</t>
+  </si>
+  <si>
+    <t>https://www.conrad.be/nl/p/tru-components-tc-mor01sj0501a10203-metaalfilmweerstand-500-axiaal-bedraad-1-w-5-1-stuk-s-1585439.html</t>
+  </si>
+  <si>
+    <t>https://www.conrad.be/nl/p/te-connectivity-2-1625890-0-metaalfilmweerstand-1-k-axiaal-bedraad-2-w-5-1-stuk-s-1676924.html</t>
+  </si>
+  <si>
+    <t>Weerstand [1000 ohm]</t>
+  </si>
+  <si>
+    <t>Weerstand [1800 ohm]</t>
+  </si>
+  <si>
+    <t>Weerstand [1200 ohm]</t>
+  </si>
+  <si>
+    <t>Weerstand [33 ohm]</t>
+  </si>
+  <si>
+    <t>Weerstand [150 ohm]</t>
+  </si>
+  <si>
+    <t>Weerstand [500 ohm]</t>
+  </si>
+  <si>
+    <t>https://www.conrad.be/nl/p/te-connectivity-5-1625892-8-metaalfilmweerstand-560-axiaal-bedraad-3-w-5-1-stuk-s-1677115.html</t>
+  </si>
+  <si>
+    <t>https://www.conrad.be/nl/p/weltron-402001-vermogensweerstand-82-axiaal-bedraad-5-w-5-1-stuk-s-402001.html</t>
+  </si>
+  <si>
+    <t>Weerstand [560 ohm]</t>
+  </si>
+  <si>
+    <t>Weerstand [82 ohm]</t>
+  </si>
+  <si>
+    <t>https://www.conrad.be/nl/p/weltron-401781-vermogensweerstand-1-2-axiaal-bedraad-5-w-5-1-stuk-s-401781.html</t>
+  </si>
+  <si>
+    <t>https://www.conrad.be/nl/p/thomsen-402168-vermogensweerstand-1-8-k-axiaal-bedraad-5-w-5-1-stuk-s-402168.html</t>
+  </si>
+  <si>
+    <t>Conrad</t>
+  </si>
+  <si>
+    <t>Farnell</t>
+  </si>
+  <si>
+    <t>Mouser</t>
   </si>
 </sst>
 </file>
@@ -188,7 +245,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -205,7 +262,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -525,14 +585,14 @@
   <dimension ref="A1:J49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:J4"/>
+      <selection activeCell="D21" sqref="D21:J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.6640625" customWidth="1"/>
+    <col min="10" max="10" width="56.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -560,204 +620,280 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="2"/>
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="D3" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="D4" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
+        <v>12</v>
+      </c>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
-      <c r="B6" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>1</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
+        <v>23</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
-      <c r="B9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="2"/>
+      <c r="A9" s="1">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="D9" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
+        <v>27</v>
+      </c>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
+      <c r="A10" s="1">
+        <v>1</v>
+      </c>
       <c r="B10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
+        <v>24</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
+      <c r="A11" s="1">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
+      <c r="A12" s="1">
+        <v>1</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
+      <c r="A13" s="1">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
+      <c r="A14" s="1">
+        <v>1</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
+      <c r="A15" s="1">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
@@ -1161,31 +1297,24 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="48">
-    <mergeCell ref="D12:J12"/>
-    <mergeCell ref="D1:J1"/>
-    <mergeCell ref="D2:J2"/>
-    <mergeCell ref="D3:J3"/>
-    <mergeCell ref="D4:J4"/>
-    <mergeCell ref="D5:J5"/>
-    <mergeCell ref="D6:J6"/>
-    <mergeCell ref="D7:J7"/>
-    <mergeCell ref="D8:J8"/>
-    <mergeCell ref="D9:J9"/>
-    <mergeCell ref="D10:J10"/>
-    <mergeCell ref="D11:J11"/>
-    <mergeCell ref="D24:J24"/>
-    <mergeCell ref="D13:J13"/>
-    <mergeCell ref="D14:J14"/>
-    <mergeCell ref="D15:J15"/>
-    <mergeCell ref="D16:J16"/>
-    <mergeCell ref="D17:J17"/>
+  <mergeCells count="34">
     <mergeCell ref="D18:J18"/>
     <mergeCell ref="D19:J19"/>
     <mergeCell ref="D20:J20"/>
     <mergeCell ref="D21:J21"/>
     <mergeCell ref="D22:J22"/>
-    <mergeCell ref="D23:J23"/>
+    <mergeCell ref="D48:J48"/>
+    <mergeCell ref="D37:J37"/>
+    <mergeCell ref="D38:J38"/>
+    <mergeCell ref="D39:J39"/>
+    <mergeCell ref="D40:J40"/>
+    <mergeCell ref="D41:J41"/>
+    <mergeCell ref="D42:J42"/>
+    <mergeCell ref="D43:J43"/>
+    <mergeCell ref="D44:J44"/>
+    <mergeCell ref="D45:J45"/>
+    <mergeCell ref="D46:J46"/>
+    <mergeCell ref="D47:J47"/>
     <mergeCell ref="D36:J36"/>
     <mergeCell ref="D25:J25"/>
     <mergeCell ref="D26:J26"/>
@@ -1198,25 +1327,28 @@
     <mergeCell ref="D33:J33"/>
     <mergeCell ref="D34:J34"/>
     <mergeCell ref="D35:J35"/>
-    <mergeCell ref="D48:J48"/>
-    <mergeCell ref="D37:J37"/>
-    <mergeCell ref="D38:J38"/>
-    <mergeCell ref="D39:J39"/>
-    <mergeCell ref="D40:J40"/>
-    <mergeCell ref="D41:J41"/>
-    <mergeCell ref="D42:J42"/>
-    <mergeCell ref="D43:J43"/>
-    <mergeCell ref="D44:J44"/>
-    <mergeCell ref="D45:J45"/>
-    <mergeCell ref="D46:J46"/>
-    <mergeCell ref="D47:J47"/>
+    <mergeCell ref="D24:J24"/>
+    <mergeCell ref="D23:J23"/>
+    <mergeCell ref="D16:J16"/>
+    <mergeCell ref="D1:J1"/>
+    <mergeCell ref="D17:J17"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D9" r:id="rId1" xr:uid="{B97D9702-9453-4039-858D-71E4E4C7D17B}"/>
-    <hyperlink ref="D4" r:id="rId2" xr:uid="{C42FE50C-2C8A-48CF-BE2C-1A8FAB07645B}"/>
-    <hyperlink ref="D3" r:id="rId3" xr:uid="{834664CF-3E45-4490-A44B-987A863455F0}"/>
+    <hyperlink ref="D7" r:id="rId1" xr:uid="{B97D9702-9453-4039-858D-71E4E4C7D17B}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{C42FE50C-2C8A-48CF-BE2C-1A8FAB07645B}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{834664CF-3E45-4490-A44B-987A863455F0}"/>
+    <hyperlink ref="D4" r:id="rId4" xr:uid="{A1B876C5-222F-4B0A-9D52-0D4890991B17}"/>
+    <hyperlink ref="D5" r:id="rId5" xr:uid="{550BC2BC-459E-4EC2-8ECD-C262BA6DB3C4}"/>
+    <hyperlink ref="D6" r:id="rId6" xr:uid="{BBD083FC-556E-4253-AA83-67AE37608A2F}"/>
+    <hyperlink ref="D8" r:id="rId7" xr:uid="{370A3CF3-E5E1-400F-97C6-75A7E2BDAC3D}"/>
+    <hyperlink ref="D10" r:id="rId8" xr:uid="{1D93BB13-3209-486B-93D5-1ECC6AB7FD7B}"/>
+    <hyperlink ref="D11" r:id="rId9" xr:uid="{DCA6A669-0510-4E33-AF58-53E559BD6FA7}"/>
+    <hyperlink ref="D13" r:id="rId10" xr:uid="{DA773582-E5D7-428F-8A54-65B3C05C94CD}"/>
+    <hyperlink ref="D12" r:id="rId11" xr:uid="{B4C9045B-2052-456F-B8D6-0F3826353601}"/>
+    <hyperlink ref="D9" r:id="rId12" xr:uid="{B806F70B-76C7-4EDA-A148-2C1C022963A1}"/>
+    <hyperlink ref="D14" r:id="rId13" xr:uid="{A88F3934-6427-4164-B93C-3A603ED92AB6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updat bill of materials
</commit_message>
<xml_diff>
--- a/Bill_of_materials_NOG NIET KLAAR.xlsx
+++ b/Bill_of_materials_NOG NIET KLAAR.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gijsj\Documents\1_EAI\Github\Elektronische-systemen-2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bomen\Documenten\School\PXL\2EAI\semester_2\ElektronischeSystemen2\Elektronische_systemen_2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76511066-1AD5-4F63-BB5A-2CD07ACDAA4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE65CA82-1A4C-432C-81F1-3D60CD32CC34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{23BF4C88-1078-42E7-9D0C-D5A36D1001D8}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="53">
   <si>
     <t>Aantal</t>
   </si>
@@ -140,6 +140,60 @@
   </si>
   <si>
     <t>Mouser</t>
+  </si>
+  <si>
+    <t>Button</t>
+  </si>
+  <si>
+    <t>Weerstand [10k ohm]</t>
+  </si>
+  <si>
+    <t>Buzzer</t>
+  </si>
+  <si>
+    <t>Alcohol sensor MQ3</t>
+  </si>
+  <si>
+    <t>LM358</t>
+  </si>
+  <si>
+    <t>LCD-16X2</t>
+  </si>
+  <si>
+    <t>BC547</t>
+  </si>
+  <si>
+    <t>https://www.conrad.be/nl/p/yageo-mf0207fte52-10k-metaalfilmweerstand-10-k-axiaal-bedraad-0207-0-6-w-1-1-stuk-s-1417569.html</t>
+  </si>
+  <si>
+    <t>KIWI elektronics</t>
+  </si>
+  <si>
+    <t>https://www.kiwi-electronics.nl/nl/alcohol-gas-sensor-mq-3-2509</t>
+  </si>
+  <si>
+    <t>Reichelt</t>
+  </si>
+  <si>
+    <t>https://www.reichelt.com/be/nl/operationele-versterker-2-voudig-dip-8-lm-358-dip-p10483.html?PROVID=2812&amp;gclid=CjwKCAiAprGRBhBgEiwANJEY7Fxc8xlu0Sk7hXjV2c4zK-R9CKrMgwO9HYf3zC9clGJQoc62MzMLMhoC0zUQAvD_BwE</t>
+  </si>
+  <si>
+    <t>https://www.conrad.be/nl/p/joy-it-com-lcd-16x2-displaymodule-6-6-cm-2-6-inch-16-x-4-pixel-geschikt-voor-serie-arduino-met-achtergrondverlichting-1656369.html</t>
+  </si>
+  <si>
+    <t xml:space="preserve">farnell </t>
+  </si>
+  <si>
+    <t>https://nl.farnell.com/on-semiconductor/bc547ctfr/transistor-bipol-npn-45v-to-92/dp/2453792RL?st=BC547</t>
+  </si>
+  <si>
+    <t>LM393</t>
+  </si>
+  <si>
+    <t>farnell</t>
+  </si>
+  <si>
+    <t>https://nl.farnell.com/stmicroelectronics/lm393dt/comparator-dual-1-3us-soic-8/dp/2382619?st=LM393</t>
   </si>
 </sst>
 </file>
@@ -245,7 +299,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -255,6 +309,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -262,9 +322,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -585,14 +648,15 @@
   <dimension ref="A1:J49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21:J21"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
     <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="56.21875" customWidth="1"/>
+    <col min="10" max="10" width="68.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -605,15 +669,15 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
@@ -625,15 +689,15 @@
       <c r="C2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
@@ -645,15 +709,15 @@
       <c r="C3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
@@ -665,15 +729,15 @@
       <c r="C4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
@@ -685,15 +749,15 @@
       <c r="C5" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
@@ -705,15 +769,15 @@
       <c r="C6" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
@@ -725,15 +789,15 @@
       <c r="C7" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
@@ -745,15 +809,15 @@
       <c r="C8" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
@@ -765,15 +829,15 @@
       <c r="C9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
@@ -785,15 +849,15 @@
       <c r="C10" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
@@ -805,15 +869,15 @@
       <c r="C11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
@@ -825,19 +889,19 @@
       <c r="C12" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B13" t="s">
         <v>20</v>
@@ -845,15 +909,15 @@
       <c r="C13" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
@@ -865,15 +929,15 @@
       <c r="C14" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
@@ -885,411 +949,467 @@
       <c r="C15" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
-      <c r="B16" s="2"/>
+      <c r="A16" s="1">
+        <v>1</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="C16" s="2"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
+      <c r="A17" s="1">
+        <v>7</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
-      <c r="B18" s="2"/>
+      <c r="A18" s="1">
+        <v>1</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>37</v>
+      </c>
       <c r="C18" s="2"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
-      <c r="J18" s="5"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="7"/>
+      <c r="J18" s="7"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
+      <c r="A19" s="1">
+        <v>1</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="10"/>
+      <c r="J19" s="10"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="1"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
+      <c r="A20" s="1">
+        <v>1</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="1"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
+      <c r="A21" s="1">
+        <v>1</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="1"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
+      <c r="A22" s="1">
+        <v>1</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" s="10"/>
+      <c r="F22" s="10"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="10"/>
+      <c r="J22" s="10"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="1"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
+      <c r="A23" s="1">
+        <v>1</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="E23" s="10"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="10"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
-      <c r="J24" s="5"/>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="7"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
-      <c r="J25" s="5"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
-      <c r="J26" s="5"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
-      <c r="I27" s="5"/>
-      <c r="J27" s="5"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
-      <c r="I28" s="5"/>
-      <c r="J28" s="5"/>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="10"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="10"/>
+      <c r="J29" s="10"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
-      <c r="I30" s="5"/>
-      <c r="J30" s="5"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="10"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="10"/>
+      <c r="J30" s="10"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
-      <c r="J31" s="5"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="7"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
-      <c r="I32" s="5"/>
-      <c r="J32" s="5"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="7"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="7"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
-      <c r="H33" s="5"/>
-      <c r="I33" s="5"/>
-      <c r="J33" s="5"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="7"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
-      <c r="I34" s="5"/>
-      <c r="J34" s="5"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="7"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
-      <c r="H35" s="5"/>
-      <c r="I35" s="5"/>
-      <c r="J35" s="5"/>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="7"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="5"/>
-      <c r="I36" s="5"/>
-      <c r="J36" s="5"/>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="7"/>
+      <c r="H36" s="7"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="7"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" s="1"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
-      <c r="H37" s="5"/>
-      <c r="I37" s="5"/>
-      <c r="J37" s="5"/>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="7"/>
+      <c r="I37" s="7"/>
+      <c r="J37" s="7"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
-      <c r="H38" s="5"/>
-      <c r="I38" s="5"/>
-      <c r="J38" s="5"/>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
+      <c r="F38" s="7"/>
+      <c r="G38" s="7"/>
+      <c r="H38" s="7"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="7"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" s="1"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
-      <c r="F39" s="5"/>
-      <c r="G39" s="5"/>
-      <c r="H39" s="5"/>
-      <c r="I39" s="5"/>
-      <c r="J39" s="5"/>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="7"/>
+      <c r="I39" s="7"/>
+      <c r="J39" s="7"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="5"/>
-      <c r="F40" s="5"/>
-      <c r="G40" s="5"/>
-      <c r="H40" s="5"/>
-      <c r="I40" s="5"/>
-      <c r="J40" s="5"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+      <c r="G40" s="7"/>
+      <c r="H40" s="7"/>
+      <c r="I40" s="7"/>
+      <c r="J40" s="7"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
-      <c r="F41" s="5"/>
-      <c r="G41" s="5"/>
-      <c r="H41" s="5"/>
-      <c r="I41" s="5"/>
-      <c r="J41" s="5"/>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
+      <c r="F41" s="7"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="7"/>
+      <c r="I41" s="7"/>
+      <c r="J41" s="7"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
-      <c r="G42" s="5"/>
-      <c r="H42" s="5"/>
-      <c r="I42" s="5"/>
-      <c r="J42" s="5"/>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
+      <c r="F42" s="7"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="7"/>
+      <c r="I42" s="7"/>
+      <c r="J42" s="7"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="5"/>
-      <c r="G43" s="5"/>
-      <c r="H43" s="5"/>
-      <c r="I43" s="5"/>
-      <c r="J43" s="5"/>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7"/>
+      <c r="G43" s="7"/>
+      <c r="H43" s="7"/>
+      <c r="I43" s="7"/>
+      <c r="J43" s="7"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5"/>
-      <c r="F44" s="5"/>
-      <c r="G44" s="5"/>
-      <c r="H44" s="5"/>
-      <c r="I44" s="5"/>
-      <c r="J44" s="5"/>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
+      <c r="F44" s="7"/>
+      <c r="G44" s="7"/>
+      <c r="H44" s="7"/>
+      <c r="I44" s="7"/>
+      <c r="J44" s="7"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" s="1"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="5"/>
-      <c r="F45" s="5"/>
-      <c r="G45" s="5"/>
-      <c r="H45" s="5"/>
-      <c r="I45" s="5"/>
-      <c r="J45" s="5"/>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7"/>
+      <c r="G45" s="7"/>
+      <c r="H45" s="7"/>
+      <c r="I45" s="7"/>
+      <c r="J45" s="7"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" s="1"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="5"/>
-      <c r="F46" s="5"/>
-      <c r="G46" s="5"/>
-      <c r="H46" s="5"/>
-      <c r="I46" s="5"/>
-      <c r="J46" s="5"/>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
+      <c r="G46" s="7"/>
+      <c r="H46" s="7"/>
+      <c r="I46" s="7"/>
+      <c r="J46" s="7"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" s="1"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="5"/>
-      <c r="F47" s="5"/>
-      <c r="G47" s="5"/>
-      <c r="H47" s="5"/>
-      <c r="I47" s="5"/>
-      <c r="J47" s="5"/>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7"/>
+      <c r="G47" s="7"/>
+      <c r="H47" s="7"/>
+      <c r="I47" s="7"/>
+      <c r="J47" s="7"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
-      <c r="D48" s="5"/>
-      <c r="E48" s="5"/>
-      <c r="F48" s="5"/>
-      <c r="G48" s="5"/>
-      <c r="H48" s="5"/>
-      <c r="I48" s="5"/>
-      <c r="J48" s="5"/>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
+      <c r="F48" s="7"/>
+      <c r="G48" s="7"/>
+      <c r="H48" s="7"/>
+      <c r="I48" s="7"/>
+      <c r="J48" s="7"/>
     </row>
     <row r="49" spans="4:4" x14ac:dyDescent="0.3">
       <c r="D49" t="s">
@@ -1298,11 +1418,23 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="D18:J18"/>
-    <mergeCell ref="D19:J19"/>
-    <mergeCell ref="D20:J20"/>
-    <mergeCell ref="D21:J21"/>
-    <mergeCell ref="D22:J22"/>
+    <mergeCell ref="D24:J24"/>
+    <mergeCell ref="D23:J23"/>
+    <mergeCell ref="D16:J16"/>
+    <mergeCell ref="D1:J1"/>
+    <mergeCell ref="D17:J17"/>
+    <mergeCell ref="D36:J36"/>
+    <mergeCell ref="D25:J25"/>
+    <mergeCell ref="D26:J26"/>
+    <mergeCell ref="D27:J27"/>
+    <mergeCell ref="D28:J28"/>
+    <mergeCell ref="D29:J29"/>
+    <mergeCell ref="D30:J30"/>
+    <mergeCell ref="D31:J31"/>
+    <mergeCell ref="D32:J32"/>
+    <mergeCell ref="D33:J33"/>
+    <mergeCell ref="D34:J34"/>
+    <mergeCell ref="D35:J35"/>
     <mergeCell ref="D48:J48"/>
     <mergeCell ref="D37:J37"/>
     <mergeCell ref="D38:J38"/>
@@ -1315,23 +1447,11 @@
     <mergeCell ref="D45:J45"/>
     <mergeCell ref="D46:J46"/>
     <mergeCell ref="D47:J47"/>
-    <mergeCell ref="D36:J36"/>
-    <mergeCell ref="D25:J25"/>
-    <mergeCell ref="D26:J26"/>
-    <mergeCell ref="D27:J27"/>
-    <mergeCell ref="D28:J28"/>
-    <mergeCell ref="D29:J29"/>
-    <mergeCell ref="D30:J30"/>
-    <mergeCell ref="D31:J31"/>
-    <mergeCell ref="D32:J32"/>
-    <mergeCell ref="D33:J33"/>
-    <mergeCell ref="D34:J34"/>
-    <mergeCell ref="D35:J35"/>
-    <mergeCell ref="D24:J24"/>
-    <mergeCell ref="D23:J23"/>
-    <mergeCell ref="D16:J16"/>
-    <mergeCell ref="D1:J1"/>
-    <mergeCell ref="D17:J17"/>
+    <mergeCell ref="D18:J18"/>
+    <mergeCell ref="D19:J19"/>
+    <mergeCell ref="D20:J20"/>
+    <mergeCell ref="D21:J21"/>
+    <mergeCell ref="D22:J22"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D7" r:id="rId1" xr:uid="{B97D9702-9453-4039-858D-71E4E4C7D17B}"/>
@@ -1347,8 +1467,14 @@
     <hyperlink ref="D12" r:id="rId11" xr:uid="{B4C9045B-2052-456F-B8D6-0F3826353601}"/>
     <hyperlink ref="D9" r:id="rId12" xr:uid="{B806F70B-76C7-4EDA-A148-2C1C022963A1}"/>
     <hyperlink ref="D14" r:id="rId13" xr:uid="{A88F3934-6427-4164-B93C-3A603ED92AB6}"/>
+    <hyperlink ref="D17" r:id="rId14" xr:uid="{9B4A1419-88BC-49B3-A890-E11DC1919536}"/>
+    <hyperlink ref="D19" r:id="rId15" xr:uid="{EDE89D0C-1AB8-4110-8A66-53993717D5BD}"/>
+    <hyperlink ref="D20" r:id="rId16" xr:uid="{6D71AA52-5D68-4B73-9B51-34EC88114769}"/>
+    <hyperlink ref="D21" r:id="rId17" xr:uid="{FB7BB4FC-AF4F-4156-8D19-76A4856072AD}"/>
+    <hyperlink ref="D22" r:id="rId18" xr:uid="{E2586FFA-02FD-4977-B9DC-6C03257CE72B}"/>
+    <hyperlink ref="D23" r:id="rId19" xr:uid="{3778A5C4-5D18-4185-88C5-2597AC49481A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId20"/>
 </worksheet>
 </file>
</xml_diff>